<commit_message>
Added cable for 4A5A2D1 APU lamp to interconnect
Added cable for 4A5A2D1 APU lamp to interconnect.
- Added 4A5A2W2P2 (SMP-02V-BC) to 4A5A2W2 cable.
- Added 4A5A2D1P1 (SMR-02V-B) to 4A5A2D1 APU LAMP.

Added connectors to Interconnect BOM
- SMR-02V-B was QTY 7; is 8
- SYM-001T-P0.6(N) was QTY 125; is 127
- SMP-02V-BC was QTY 7; is 8
- SHF-001T-0.8BS was QTY 134; is 136

Generated files for release folder
</commit_message>
<xml_diff>
--- a/ECAD/interconnects/reference/OH-PL-INTERCONNECT_A_v5.xlsx
+++ b/ECAD/interconnects/reference/OH-PL-INTERCONNECT_A_v5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\OpenHornet\ECAD\interconnects\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251650B0-3021-495E-9C42-BA2E1F253829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C470305D-13E1-4619-809A-10CAAAB0CD64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,18 +551,12 @@
     <t>CONN, PLUG, HSG, 2POS, 2.50MM, JST SM</t>
   </si>
   <si>
-    <t>3A2A1W1J3, 3A2A1W2J1, 3A2A1W2J2, 4A4A2W1J1, 4A4A2W1J2, 4A7A2W1J2, 5A2W1P7</t>
-  </si>
-  <si>
     <t>SMR-02V-B</t>
   </si>
   <si>
     <t>CONN, RCPT, HSG, 2POS, 2.50MM, JST SM</t>
   </si>
   <si>
-    <t>3A2A1W4P1, 3A2A1W5P1, 3A2A1W6P1, 4A4A3W1P1, 4A8A2W1P1, 4A8A3W1P1, 5A2A3W1J1</t>
-  </si>
-  <si>
     <t>PHR-6</t>
   </si>
   <si>
@@ -719,18 +713,12 @@
     <t>CONN, 22-28AWG, MALE, CRIMP TIN</t>
   </si>
   <si>
-    <t>2A2A1A3W1J1, 2A2A1A3W1J?, 2A5A1W3J1, 2A10W1P1, 2A13W3P1, 2A15W2P2, 3A2A1W3P1, 3A2A1W4P1, 3A2A1W5P1, 3A2A1W6P1, 4A2A1A2W1P1, 4A3A2W1P1, 4A4A1W1P1, 4A4A3W1P1, 4A5A2W2P1, 4A7A3W1P1, 4A7A4J1, 4A8A1W1P1, 4A8A2W1P1, 4A8A3W1P1, 4A10W1P1, 5A2A1W1J1, 5A2A2W1J1, 5A2A3W1J1, 5A5A2W1J1, 5A10A1W1J1, 5A10A2W1J1, 10A1A1W1P1, 10A1A1W2P1</t>
-  </si>
-  <si>
     <t>SHF-001T-0.8BS</t>
   </si>
   <si>
     <t>CONN, 22-28AWG, FEMALE, CRIMP TIN</t>
   </si>
   <si>
-    <t>2A2A1W1P7, 2A4A1W2P5, 2A5A1W1P6, 2A12A1W5J2, 2A12A1W5J3, 2A12A1W5J4, 2A13W3J1, 3A2A1W1J1, 3A2A1W1J2, 3A2A1W1J3, 3A2A1W2J1, 3A2A1W2J2, 4A2A1W1J1, 4A3A3W1J1, 4A3A3W2J1, 4A4A2W1J1, 4A4A2W1J2, 4A5A2W1J1, 4A5A2W1J2, 4A7A1W3J1, 4A7A2W1J1, 4A7A2W1J2, 4A13A1W5J2, 4A13A1W5J3, 4A13A1W5J4, 5A2W1P7, 5A2W1P8, 5A2W1P9, 5A10W1P5, 5A10W1P6, 5A10W1P7</t>
-  </si>
-  <si>
     <t>39-00-0083</t>
   </si>
   <si>
@@ -831,6 +819,18 @@
   </si>
   <si>
     <t>1A1W6P3, 1A2W1P3, 1A6W1P3, 1A7W1P3, 1A7W2P4, 1A8A1W1P1, 1A8W2P1, 1A8W3P1, 1A8W4P1, 1A8W5P1, 1A8W5P2, 1A8W7P1, 1A8W8P1, 1A8W9P1, 2A2A1W1P3, 2A2A1W1P4, 2A2A1W1P5, 2A2A1W1P6, 2A3A1W1P2, 2A4A1W1P3, 2A4A1W1P4, 2A4A1W2P4, 2A5A1W1P4, 2A5A1W2P3, 2A5A1W2P4, 2A5A1W2P5, 2A5A1W2P6, 2A7A1A1SW1P1, 2A7A1A1SW2P1, 2A7A1A2RV1P1, 2A7A1A4SW1P1, 2A7A1W1P1, 2A7A1W1P2, 2A7A1W1P3, 2A7A1W1P4, 2A7A1W2P1, 2A7A1W2P2, 2A7A1W3P1, 2A7A1W3P2, 2A7A1W3P3, 2A7A1W3P4, 2A15W2P1, 2A15W3P1, 2A15W3P2, 3A2A1W1P3, 3A2A1W2P4, 4A1W11P6, 4A2A1W1P3, 4A3A1W1P3, 4A3A1W2P4, 4A3A3W1P3, 4A3A3W2P4, 4A3A3W2P6, 4A4A2W1P3, 4A5A1A1W1P1, 4A5A2W1P4, 4A6A1W1P4, 4A7A1W1P4, 4A7A1W2P6, 4A7A1W3P3, 4A7A2W1P1, 5A2A4W1P1, 5A2A4W2P1, 5A2A4W3P1, 5A2A4W4P1, 5A2A4W5P1, 5A2A4W6P1, 5A2A4W6P2, 5A2A4W6P3, 5A2A4W6P4, 5A2W1P1, 5A2W1P3, 5A2W1P4, 5A2W1P6, 5A4A1W1P3, 5A4A1W2P3, 5A5A1W1P3, 5A4W1P1, 5A5A1W2P4, 5A6A1P3, 5A6A1P4, 5A7A1W1P3, 5A7A1W2P4, 5A8A1W1P3, 5A8A1W2P4, 5A9A1W1P3, 5A9A1W2P4, 5A10W1P3, 5A10W1P4</t>
+  </si>
+  <si>
+    <t>2A2A1A3W1J1, 2A2A1A3W1J?, 2A5A1W3J1, 2A10W1P1, 2A13W3P1, 2A15W2P2, 3A2A1W3P1, 3A2A1W4P1, 3A2A1W5P1, 3A2A1W6P1, 4A2A1A2W1P1, 4A3A2W1P1, 4A4A1W1P1, 4A4A3W1P1, 4A5A2W2P1, 4A5A2D1P1, 4A7A3W1P1, 4A7A4J1, 4A8A1W1P1, 4A8A2W1P1, 4A8A3W1P1, 4A10W1P1, 5A2A1W1J1, 5A2A2W1J1, 5A2A3W1J1, 5A5A2W1J1, 5A10A1W1J1, 5A10A2W1J1, 10A1A1W1P1, 10A1A1W2P1</t>
+  </si>
+  <si>
+    <t>3A2A1W4P1, 3A2A1W5P1, 3A2A1W6P1, 4A4A3W1P1, 4A5A2D1P1, 4A8A2W1P1, 4A8A3W1P1, 5A2A3W1J1</t>
+  </si>
+  <si>
+    <t>2A2A1W1P7, 2A4A1W2P5, 2A5A1W1P6, 2A12A1W5J2, 2A12A1W5J3, 2A12A1W5J4, 2A13W3J1, 3A2A1W1J1, 3A2A1W1J2, 3A2A1W1J3, 3A2A1W2J1, 3A2A1W2J2, 4A2A1W1J1, 4A3A3W1J1, 4A3A3W2J1, 4A4A2W1J1, 4A4A2W1J2, 4A5A2W1J1, 4A5A2W1J2, 4A5A2W2P2, 4A7A1W3J1, 4A7A2W1J1, 4A7A2W1J2, 4A13A1W5J2, 4A13A1W5J3, 4A13A1W5J4, 5A2W1P7, 5A2W1P8, 5A2W1P9, 5A10W1P5, 5A10W1P6, 5A10W1P7</t>
+  </si>
+  <si>
+    <t>3A2A1W1J3, 3A2A1W2J1, 3A2A1W2J2, 4A4A2W1J1, 4A4A2W1J2, 4A5A2W2P2, 4A7A2W1J2, 5A2W1P7</t>
   </si>
 </sst>
 </file>
@@ -1999,7 +1999,7 @@
   <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2012,69 +2012,69 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C1" s="17"/>
       <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C2" s="17"/>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C3" s="17"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>250</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>254</v>
       </c>
       <c r="C4" s="17"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C5" s="17"/>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2088,10 +2088,10 @@
         <v>3814</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2102,7 +2102,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>40</v>
@@ -2119,7 +2119,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>42</v>
@@ -2136,7 +2136,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>48</v>
@@ -2153,7 +2153,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>46</v>
@@ -2170,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>162</v>
@@ -2187,13 +2187,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>203</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2204,13 +2204,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>209</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2272,13 +2272,13 @@
         <v>1</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2289,10 +2289,10 @@
         <v>66</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>126</v>
@@ -2306,10 +2306,10 @@
         <v>8</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>149</v>
@@ -2323,10 +2323,10 @@
         <v>2</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>99</v>
@@ -2340,10 +2340,10 @@
         <v>8</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>137</v>
@@ -2357,10 +2357,10 @@
         <v>44</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>15</v>
@@ -2374,13 +2374,13 @@
         <v>12</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2510,13 +2510,13 @@
         <v>73</v>
       </c>
       <c r="C32" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>223</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2561,13 +2561,13 @@
         <v>1</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2578,13 +2578,13 @@
         <v>1</v>
       </c>
       <c r="C36" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>188</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2748,13 +2748,13 @@
         <v>1</v>
       </c>
       <c r="C46" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E46" s="15" t="s">
         <v>200</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2782,13 +2782,13 @@
         <v>1</v>
       </c>
       <c r="C48" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E48" s="15" t="s">
         <v>213</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2816,13 +2816,13 @@
         <v>1</v>
       </c>
       <c r="C50" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E50" s="15" t="s">
         <v>182</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2833,13 +2833,13 @@
         <v>1</v>
       </c>
       <c r="C51" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E51" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2975,7 +2975,7 @@
         <v>66</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3009,7 +3009,7 @@
         <v>45</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3037,13 +3037,13 @@
         <v>3</v>
       </c>
       <c r="C63" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E63" s="15" t="s">
         <v>194</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="E63" s="15" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="165" x14ac:dyDescent="0.25">
@@ -3055,13 +3055,13 @@
         <v>749</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3157,13 +3157,13 @@
         <v>14</v>
       </c>
       <c r="C70" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E70" s="15" t="s">
         <v>191</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E70" s="15" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3174,13 +3174,13 @@
         <v>4</v>
       </c>
       <c r="C71" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E71" s="15" t="s">
         <v>197</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="E71" s="15" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3208,13 +3208,13 @@
         <v>4</v>
       </c>
       <c r="C73" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E73" s="15" t="s">
         <v>179</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="E73" s="15" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3225,13 +3225,13 @@
         <v>9</v>
       </c>
       <c r="C74" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E74" s="15" t="s">
         <v>176</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E74" s="15" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3256,16 +3256,16 @@
         <v>70</v>
       </c>
       <c r="B76" s="5">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>231</v>
+        <v>264</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3273,7 +3273,7 @@
         <v>71</v>
       </c>
       <c r="B77" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>170</v>
@@ -3282,7 +3282,7 @@
         <v>171</v>
       </c>
       <c r="E77" s="15" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3358,16 +3358,16 @@
         <v>76</v>
       </c>
       <c r="B82" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C82" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D82" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D82" s="6" t="s">
-        <v>174</v>
-      </c>
       <c r="E82" s="15" t="s">
-        <v>175</v>
+        <v>263</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3446,13 +3446,13 @@
         <v>134</v>
       </c>
       <c r="C87" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E87" s="15" t="s">
         <v>220</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="E87" s="15" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3460,16 +3460,16 @@
         <v>82</v>
       </c>
       <c r="B88" s="5">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E88" s="15" t="s">
-        <v>228</v>
+        <v>262</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>